<commit_message>
add evaluation metrics to report
</commit_message>
<xml_diff>
--- a/data/report.xlsx
+++ b/data/report.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\Documents\GitHub\Dissertation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0D73E4-21DF-4565-84A1-E16B391A788D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777E3081-F23A-472E-9D9D-4802D36B1F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{0F19C5E3-3E30-4E8C-BB92-BC560516A7CC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{0F19C5E3-3E30-4E8C-BB92-BC560516A7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="variable selection models" sheetId="1" r:id="rId1"/>
     <sheet name="unit root tests" sheetId="2" r:id="rId2"/>
+    <sheet name="evaluation metrics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="37">
   <si>
     <t>Lasso</t>
   </si>
@@ -115,6 +116,36 @@
   </si>
   <si>
     <t>UNIT ROOT TEST: 1st DIFFERENCE SERIES</t>
+  </si>
+  <si>
+    <t>LASSO</t>
+  </si>
+  <si>
+    <t>Adaptive LASSO</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VADER as a </t>
+  </si>
+  <si>
+    <t>regressor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM-AS-2020 as a </t>
+  </si>
+  <si>
+    <t>Minimum VADER</t>
+  </si>
+  <si>
+    <t>Minimum LA-AS-2020</t>
   </si>
 </sst>
 </file>
@@ -145,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -193,11 +224,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -205,15 +245,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,18 +594,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.5">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
@@ -814,21 +859,21 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
@@ -1051,18 +1096,18 @@
       </c>
     </row>
     <row r="25" spans="2:11" ht="21" x14ac:dyDescent="0.5">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
@@ -1315,21 +1360,21 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5" t="s">
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5" t="s">
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
@@ -1547,11 +1592,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B25:K25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="I26:K26"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="I35:K35"/>
@@ -1561,6 +1601,11 @@
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="I13:K13"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="I26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1571,7 +1616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C71D0AB-F959-4639-8F56-5B9E03EB6B5F}">
   <dimension ref="B2:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -1586,19 +1631,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C3" s="4" t="s">
@@ -1835,57 +1880,57 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
+      <c r="H17" s="7"/>
+      <c r="I17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5" t="s">
+      <c r="J17" s="7"/>
+      <c r="K17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="5"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
@@ -2111,4 +2156,1391 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B72B397-E9ED-4446-ABEE-887F641F952C}">
+  <dimension ref="C4:L29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="18.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>1.644962</v>
+      </c>
+      <c r="E6">
+        <v>4.0885749999999996</v>
+      </c>
+      <c r="F6">
+        <v>2.0220220000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.209345</v>
+      </c>
+      <c r="H6">
+        <v>7.54084E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.27460590000000001</v>
+      </c>
+      <c r="J6">
+        <v>0.176985</v>
+      </c>
+      <c r="K6">
+        <v>4.0707750000000001E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.20176160000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>1.6558630000000001</v>
+      </c>
+      <c r="E7">
+        <v>4.1696530000000003</v>
+      </c>
+      <c r="F7">
+        <v>2.041973</v>
+      </c>
+      <c r="G7">
+        <v>0.20793719999999999</v>
+      </c>
+      <c r="H7">
+        <v>6.4617850000000004E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.25420039999999999</v>
+      </c>
+      <c r="J7">
+        <v>0.1885059</v>
+      </c>
+      <c r="K7">
+        <v>4.6849259999999997E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.2164469</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1.652102</v>
+      </c>
+      <c r="E8">
+        <v>4.1453030000000002</v>
+      </c>
+      <c r="F8">
+        <v>2.0360019999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.2071393</v>
+      </c>
+      <c r="H8">
+        <v>7.3337579999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>0.27080910000000002</v>
+      </c>
+      <c r="J8">
+        <v>0.18141460000000001</v>
+      </c>
+      <c r="K8">
+        <v>4.294328E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.20722760000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>0.18138779999999999</v>
+      </c>
+      <c r="E11">
+        <v>5.3060419999999997E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.23034850000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.70233599999999996</v>
+      </c>
+      <c r="H11">
+        <v>0.75246500000000005</v>
+      </c>
+      <c r="I11">
+        <v>0.86744739999999998</v>
+      </c>
+      <c r="J11">
+        <v>0.45479849999999999</v>
+      </c>
+      <c r="K11">
+        <v>0.3187178</v>
+      </c>
+      <c r="L11">
+        <v>0.56455100000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>0.19606119999999999</v>
+      </c>
+      <c r="E12">
+        <v>6.0466829999999999E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.24590000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.65772419999999998</v>
+      </c>
+      <c r="H12">
+        <v>0.60244089999999995</v>
+      </c>
+      <c r="I12">
+        <v>0.77617069999999999</v>
+      </c>
+      <c r="J12">
+        <v>0.46246409999999999</v>
+      </c>
+      <c r="K12">
+        <v>0.30339050000000001</v>
+      </c>
+      <c r="L12">
+        <v>0.55080899999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.19179689999999999</v>
+      </c>
+      <c r="E13" s="9">
+        <v>5.697522E-2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.23869480000000001</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.70149870000000003</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0.77011669999999999</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.87756290000000003</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.45946310000000001</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0.33435819999999999</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0.57823720000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>1.642914</v>
+      </c>
+      <c r="E16">
+        <v>4.1823790000000001</v>
+      </c>
+      <c r="F16">
+        <v>2.0450870000000001</v>
+      </c>
+      <c r="G16">
+        <v>0.21075060000000001</v>
+      </c>
+      <c r="H16">
+        <v>7.7129900000000001E-2</v>
+      </c>
+      <c r="I16">
+        <v>0.27772269999999999</v>
+      </c>
+      <c r="J16">
+        <v>0.2053074</v>
+      </c>
+      <c r="K16">
+        <v>5.6161139999999998E-2</v>
+      </c>
+      <c r="L16">
+        <v>0.23698340000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>1.646387</v>
+      </c>
+      <c r="E17">
+        <v>4.2630319999999999</v>
+      </c>
+      <c r="F17">
+        <v>2.064711</v>
+      </c>
+      <c r="G17">
+        <v>0.23206579999999999</v>
+      </c>
+      <c r="H17">
+        <v>9.5509060000000007E-2</v>
+      </c>
+      <c r="I17">
+        <v>0.30904540000000003</v>
+      </c>
+      <c r="J17">
+        <v>0.19519529999999999</v>
+      </c>
+      <c r="K17">
+        <v>5.0856520000000002E-2</v>
+      </c>
+      <c r="L17">
+        <v>0.22551389999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1.6393470000000001</v>
+      </c>
+      <c r="E18">
+        <v>4.1682779999999999</v>
+      </c>
+      <c r="F18">
+        <v>2.041636</v>
+      </c>
+      <c r="G18">
+        <v>0.21425350000000001</v>
+      </c>
+      <c r="H18">
+        <v>7.8190019999999999E-2</v>
+      </c>
+      <c r="I18">
+        <v>0.27962480000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.2005353</v>
+      </c>
+      <c r="K18">
+        <v>5.2867579999999997E-2</v>
+      </c>
+      <c r="L18">
+        <v>0.22992950000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21">
+        <v>0.1744935</v>
+      </c>
+      <c r="E21">
+        <v>5.0767279999999998E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.22531590000000001</v>
+      </c>
+      <c r="G21">
+        <v>0.72727470000000005</v>
+      </c>
+      <c r="H21">
+        <v>0.83039969999999996</v>
+      </c>
+      <c r="I21">
+        <v>0.91126269999999998</v>
+      </c>
+      <c r="J21">
+        <v>0.46128039999999998</v>
+      </c>
+      <c r="K21">
+        <v>0.31085360000000001</v>
+      </c>
+      <c r="L21">
+        <v>0.55754250000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>0.177868</v>
+      </c>
+      <c r="E22">
+        <v>5.3939639999999997E-2</v>
+      </c>
+      <c r="F22">
+        <v>0.23224910000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.69151229999999997</v>
+      </c>
+      <c r="H22">
+        <v>0.6680294</v>
+      </c>
+      <c r="I22">
+        <v>0.81733069999999997</v>
+      </c>
+      <c r="J22">
+        <v>0.45303169999999998</v>
+      </c>
+      <c r="K22">
+        <v>0.28921019999999997</v>
+      </c>
+      <c r="L22">
+        <v>0.53778269999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>0.1745457</v>
+      </c>
+      <c r="E23">
+        <v>5.1766439999999997E-2</v>
+      </c>
+      <c r="F23">
+        <v>0.22752240000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.72767150000000003</v>
+      </c>
+      <c r="H23">
+        <v>0.86372040000000005</v>
+      </c>
+      <c r="I23">
+        <v>0.92936560000000001</v>
+      </c>
+      <c r="J23">
+        <v>0.46520929999999999</v>
+      </c>
+      <c r="K23">
+        <v>0.32615549999999999</v>
+      </c>
+      <c r="L23">
+        <v>0.57110019999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="10">
+        <f>MIN(D6:D8)</f>
+        <v>1.644962</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" ref="E25:L25" si="0">MIN(E6:E8)</f>
+        <v>4.0885749999999996</v>
+      </c>
+      <c r="F25" s="10">
+        <f t="shared" si="0"/>
+        <v>2.0220220000000002</v>
+      </c>
+      <c r="G25" s="10">
+        <f t="shared" si="0"/>
+        <v>0.2071393</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="0"/>
+        <v>6.4617850000000004E-2</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="0"/>
+        <v>0.25420039999999999</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="0"/>
+        <v>0.176985</v>
+      </c>
+      <c r="K25" s="10">
+        <f t="shared" si="0"/>
+        <v>4.0707750000000001E-2</v>
+      </c>
+      <c r="L25" s="10">
+        <f t="shared" si="0"/>
+        <v>0.20176160000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="10">
+        <f>MIN(D16:D18)</f>
+        <v>1.6393470000000001</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" ref="E26:L26" si="1">MIN(E16:E18)</f>
+        <v>4.1682779999999999</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="1"/>
+        <v>2.041636</v>
+      </c>
+      <c r="G26" s="10">
+        <f t="shared" si="1"/>
+        <v>0.21075060000000001</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="1"/>
+        <v>7.7129900000000001E-2</v>
+      </c>
+      <c r="I26" s="10">
+        <f t="shared" si="1"/>
+        <v>0.27772269999999999</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" si="1"/>
+        <v>0.19519529999999999</v>
+      </c>
+      <c r="K26" s="10">
+        <f t="shared" si="1"/>
+        <v>5.0856520000000002E-2</v>
+      </c>
+      <c r="L26" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22551389999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="D27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="10">
+        <f>MIN(D11:D13)</f>
+        <v>0.18138779999999999</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" ref="E28:L28" si="2">MIN(E11:E13)</f>
+        <v>5.3060419999999997E-2</v>
+      </c>
+      <c r="F28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.23034850000000001</v>
+      </c>
+      <c r="G28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.65772419999999998</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.60244089999999995</v>
+      </c>
+      <c r="I28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.77617069999999999</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.45479849999999999</v>
+      </c>
+      <c r="K28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.30339050000000001</v>
+      </c>
+      <c r="L28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.55080899999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="10">
+        <f>MIN(D21:D23)</f>
+        <v>0.1744935</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" ref="E29:L29" si="3">MIN(E21:E23)</f>
+        <v>5.0767279999999998E-2</v>
+      </c>
+      <c r="F29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.22531590000000001</v>
+      </c>
+      <c r="G29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.69151229999999997</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.6680294</v>
+      </c>
+      <c r="I29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.81733069999999997</v>
+      </c>
+      <c r="J29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.45303169999999998</v>
+      </c>
+      <c r="K29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.28921019999999997</v>
+      </c>
+      <c r="L29" s="10">
+        <f t="shared" si="3"/>
+        <v>0.53778269999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:L9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6:D8">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:E8">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F8">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G8">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H8">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I8">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:J8">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:K8">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6:L8">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D18">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D13">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E13">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F13">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G13">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:H13">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I13">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J13">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11:K13">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11:L13">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:E18">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:F18">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16:G18">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:H18">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:I18">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:J18">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16:K18">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16:L18">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D23">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21:E23">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:F23">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21:G23">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21:H23">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21:I23">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21:J23">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:K23">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:L23">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:L26">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:L29">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D29">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:E29">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28:F29">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28:G29">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28:H29">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:I29">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28:J29">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:K29">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L28:L29">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:D26">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E26">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:F26">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:G26">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:H26">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25:I26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25:J26">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25:K26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L25:L26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>